<commit_message>
submitted by zerui 230329
</commit_message>
<xml_diff>
--- a/paper/21cm intensity mapping/parameters of surveys.xlsx
+++ b/paper/21cm intensity mapping/parameters of surveys.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LRayleighJ\NAOC\WORK\paper\21cm intensity mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B2D1FC-E7A0-433F-BA7E-1F8CCC2D8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F2AE57-3E21-4744-B200-6011DC7A5946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16185" yWindow="4815" windowWidth="10230" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16185" yWindow="4815" windowWidth="10230" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>FAST</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +73,50 @@
   </si>
   <si>
     <t>FAST_wideband</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$\sigma_{\omega_0}$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$\sigma_{\omega_a}$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST_Lband</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeerKAT_b1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeerKAT_b2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST zmin=0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST zmin=0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST zmin=0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST zmin=0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST wideband</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAST wb($T_sys=20K$)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -408,6 +453,8 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="3" max="3" width="18.25" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -415,13 +462,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -429,12 +476,12 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>20000</v>
+        <v>100000</v>
+      </c>
+      <c r="C2">
+        <v>4000</v>
       </c>
       <c r="D2">
-        <v>4000</v>
-      </c>
-      <c r="E2">
         <v>4000</v>
       </c>
     </row>
@@ -446,13 +493,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>64</v>
       </c>
       <c r="E3">
-        <v>64</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -480,13 +527,13 @@
         <v>300</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>13.5</v>
       </c>
       <c r="D5">
         <v>13.5</v>
       </c>
       <c r="E5">
-        <v>13.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -497,13 +544,13 @@
         <v>20</v>
       </c>
       <c r="C6">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
         <v>60</v>
-      </c>
-      <c r="D6">
-        <v>29</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -514,13 +561,13 @@
         <v>400</v>
       </c>
       <c r="C7">
+        <v>435</v>
+      </c>
+      <c r="D7">
+        <v>520</v>
+      </c>
+      <c r="E7">
         <v>780</v>
-      </c>
-      <c r="D7">
-        <v>435</v>
-      </c>
-      <c r="E7">
-        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -531,13 +578,13 @@
         <v>1360</v>
       </c>
       <c r="C8">
+        <v>1015</v>
+      </c>
+      <c r="D8">
+        <v>1420</v>
+      </c>
+      <c r="E8">
         <v>1050</v>
-      </c>
-      <c r="D8">
-        <v>1015</v>
-      </c>
-      <c r="E8">
-        <v>1420</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -547,11 +594,140 @@
       <c r="B9">
         <v>20000</v>
       </c>
+      <c r="C9">
+        <v>4000</v>
+      </c>
       <c r="D9">
         <v>4000</v>
       </c>
-      <c r="E9">
-        <v>4000</v>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A03DCC-6FB5-4B4C-BC5F-3705693BCCF6}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.46889999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0.30359999999999998</v>
+      </c>
+      <c r="C4">
+        <v>1.0204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>0.182</v>
+      </c>
+      <c r="C5">
+        <v>0.73140000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>9.2700000000000005E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.30470000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>6.0299999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.1832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.1376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1.1732</v>
+      </c>
+      <c r="C9">
+        <v>3.5682</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>0.23649999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.69750000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>